<commit_message>
[ADD] Implement the creation of carbon factor
</commit_message>
<xml_diff>
--- a/mycityco2_data_process/data/common/carbon_factor_mapping.xlsx
+++ b/mycityco2_data_process/data/common/carbon_factor_mapping.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4713" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="458">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -568,6 +568,12 @@
     <t xml:space="preserve">Wool, silk-worm cocoons</t>
   </si>
   <si>
+    <t xml:space="preserve">carbon_factor.null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -812,9 +818,6 @@
   </si>
   <si>
     <t xml:space="preserve">Facteur d'emission 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carbon_factor.null</t>
   </si>
   <si>
     <t xml:space="preserve">Financial intermediation services (except insurance and pension funding services)</t>
@@ -1554,13 +1557,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2120"/>
+  <dimension ref="A1:D2121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2096" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2121" activeCellId="0" sqref="A2121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53"/>
@@ -33363,6 +33366,20 @@
       </c>
       <c r="D2120" s="0" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2121" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2121" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2121" s="0" t="n">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>
@@ -33389,7 +33406,7 @@
       <selection pane="topLeft" activeCell="A313" activeCellId="0" sqref="A313"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="100.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="129.14"/>
@@ -33397,35 +33414,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0.4033</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1.2705</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33436,7 +33453,7 @@
         <v>0.4009</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33447,40 +33464,40 @@
         <v>2.6795</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>3.7602</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>0.7751</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33491,7 +33508,7 @@
         <v>0.3487</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33502,7 +33519,7 @@
         <v>0.4033</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33513,7 +33530,7 @@
         <v>0.4985</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33524,7 +33541,7 @@
         <v>0.4032</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33535,29 +33552,29 @@
         <v>1.2558</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>0.4984</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>0.5769</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33568,18 +33585,18 @@
         <v>4.602</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>1.0684</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33590,62 +33607,62 @@
         <v>0.5112</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>1.0522</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>0.314</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>0.4021</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>12.1474</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>12.1474</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33656,40 +33673,40 @@
         <v>0.4975</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>0.1276</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>0.0807</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>0.2332</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33700,29 +33717,29 @@
         <v>0.6668</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>0.3909</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>2.1257</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33733,205 +33750,205 @@
         <v>0.9808</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>0.7404</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>0.4987</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>0.0656</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>0.2217</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>0.4618</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>0.4322</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>4.694</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>1.8174</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>0.1753</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B41" s="4" t="n">
         <v>0.19</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B42" s="4" t="n">
         <v>1.4679</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B43" s="4" t="n">
         <v>0.6654</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B44" s="4" t="n">
         <v>0.1738</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B45" s="4" t="n">
         <v>0.5673</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B46" s="4" t="n">
         <v>0.2634</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B47" s="4" t="n">
         <v>0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B48" s="4" t="n">
         <v>0.089</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B49" s="4" t="n">
         <v>0.3248</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33942,18 +33959,18 @@
         <v>0.5811</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B51" s="4" t="n">
         <v>0.4741</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33964,7 +33981,7 @@
         <v>0.1751</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33975,7 +33992,7 @@
         <v>1.0307</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33986,7 +34003,7 @@
         <v>0.2077</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33997,7 +34014,7 @@
         <v>6.3719</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34008,7 +34025,7 @@
         <v>1.1319</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34019,40 +34036,40 @@
         <v>0.5763</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B58" s="4" t="n">
         <v>0.1881</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B59" s="4" t="n">
         <v>0.5293</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B60" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34063,40 +34080,40 @@
         <v>0.4039</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B62" s="4" t="n">
         <v>0.058</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B63" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B64" s="4" t="n">
         <v>0.1015</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34107,7 +34124,7 @@
         <v>0.1925</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34118,18 +34135,18 @@
         <v>6.3186</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B67" s="4" t="n">
         <v>0.1066</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34140,7 +34157,7 @@
         <v>0.8457</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34151,51 +34168,51 @@
         <v>1.2558</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B70" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B71" s="4" t="n">
         <v>0.5703</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B72" s="4" t="n">
         <v>0.2112</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B73" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34206,128 +34223,128 @@
         <v>1.2558</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B75" s="4" t="n">
         <v>0.2139</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B76" s="4" t="n">
         <v>2.319</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B77" s="4" t="n">
         <v>1.9454</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B78" s="4" t="n">
         <v>0.4784</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B79" s="4" t="n">
         <v>0.3829</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B80" s="4" t="n">
         <v>0.3464</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B81" s="4" t="n">
         <v>0.1817</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B82" s="4" t="n">
         <v>0.1031</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B83" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B84" s="4" t="n">
         <v>0.2422</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B85" s="4" t="n">
         <v>0.6799</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34338,40 +34355,40 @@
         <v>1.2558</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B87" s="4" t="n">
         <v>4.0035</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B88" s="4" t="n">
         <v>4.0035</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B89" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34382,18 +34399,18 @@
         <v>0.2777</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B91" s="4" t="n">
         <v>0.1278</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34404,7 +34421,7 @@
         <v>1.4252</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34415,29 +34432,29 @@
         <v>0.267</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B94" s="4" t="n">
         <v>1.8322</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B95" s="4" t="n">
         <v>0.0917</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34448,62 +34465,62 @@
         <v>0.0979</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B97" s="4" t="n">
         <v>0.8395</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B98" s="4" t="n">
         <v>0.3778</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B99" s="4" t="n">
         <v>0.5683</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B100" s="4" t="n">
         <v>0.0614</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B101" s="4" t="n">
         <v>0.2152</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34514,40 +34531,40 @@
         <v>1.1805</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B103" s="4" t="n">
         <v>0.0689</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B104" s="4" t="n">
         <v>0.996</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B105" s="4" t="n">
         <v>0.265</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34558,7 +34575,7 @@
         <v>0.3326</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34569,7 +34586,7 @@
         <v>0.2469</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34580,7 +34597,7 @@
         <v>3.395</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34591,7 +34608,7 @@
         <v>0.1764</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34602,40 +34619,40 @@
         <v>0.2068</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B111" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B112" s="4" t="n">
         <v>1.8364</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B113" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34646,18 +34663,18 @@
         <v>0.8548</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B115" s="4" t="n">
         <v>0.2311</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34668,7 +34685,7 @@
         <v>0.8445</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34679,29 +34696,29 @@
         <v>0.779</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B118" s="4" t="n">
         <v>0.2878</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B119" s="4" t="n">
         <v>0.0691</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34712,7 +34729,7 @@
         <v>0.6203</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34723,29 +34740,29 @@
         <v>0.6982</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B122" s="4" t="n">
         <v>0.1425</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B123" s="4" t="n">
         <v>0.0051</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34756,29 +34773,29 @@
         <v>0.1156</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B125" s="4" t="n">
         <v>0.3231</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B126" s="4" t="n">
         <v>0.101</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34789,18 +34806,18 @@
         <v>0.2922</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B128" s="4" t="n">
         <v>0.1819</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34811,7 +34828,7 @@
         <v>0.8256</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34822,117 +34839,117 @@
         <v>2.5494</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B131" s="4" t="n">
         <v>0.0344</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B132" s="4" t="n">
         <v>0.176</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B133" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B134" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B135" s="4" t="n">
         <v>0.1086</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B136" s="4" t="n">
         <v>0.1321</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B137" s="4" t="n">
         <v>0.0349</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B138" s="4" t="n">
         <v>0.2602</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B139" s="4" t="n">
         <v>0.1736</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B140" s="4" t="n">
         <v>0.0539</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34943,7 +34960,7 @@
         <v>1.0934</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34954,18 +34971,18 @@
         <v>1.8088</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B143" s="4" t="n">
         <v>0.1158</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34976,18 +34993,18 @@
         <v>0.184</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B145" s="4" t="n">
         <v>1.8574</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34998,7 +35015,7 @@
         <v>0.7717</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35009,40 +35026,40 @@
         <v>0.3251</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B148" s="4" t="n">
         <v>1.0346</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B149" s="4" t="n">
         <v>0.2289</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B150" s="4" t="n">
         <v>0.2508</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35053,7 +35070,7 @@
         <v>0.8736</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35064,29 +35081,29 @@
         <v>0.9492</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B153" s="4" t="n">
         <v>0.1009</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B154" s="4" t="n">
         <v>0.7241</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35097,40 +35114,40 @@
         <v>5.8281</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="4" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B156" s="4" t="n">
         <v>0.2491</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B157" s="4" t="n">
         <v>0.2275</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B158" s="4" t="n">
         <v>0.2085</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35141,40 +35158,40 @@
         <v>1.054</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B160" s="4" t="n">
         <v>1.2558</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B161" s="4" t="n">
         <v>0.0662</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B162" s="4" t="n">
         <v>0.1899</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35185,7 +35202,7 @@
         <v>0.2055</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35196,29 +35213,29 @@
         <v>0.9078</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B165" s="4" t="n">
         <v>46.4605</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B166" s="4" t="n">
         <v>0</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -35243,7 +35260,7 @@
       <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="111"/>
@@ -35259,7 +35276,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35267,7 +35284,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35275,7 +35292,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35283,7 +35300,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35291,7 +35308,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35299,7 +35316,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35334,7 +35351,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35342,7 +35359,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35350,7 +35367,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35358,7 +35375,7 @@
         <v>72</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35366,7 +35383,7 @@
         <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35374,7 +35391,7 @@
         <v>78</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35382,7 +35399,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35399,7 +35416,7 @@
         <v>89</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35407,7 +35424,7 @@
         <v>92</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35415,7 +35432,7 @@
         <v>93</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35423,7 +35440,7 @@
         <v>95</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35449,7 +35466,7 @@
         <v>111</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35466,7 +35483,7 @@
         <v>130</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35492,7 +35509,7 @@
         <v>136</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35500,7 +35517,7 @@
         <v>141</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35508,7 +35525,7 @@
         <v>143</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35525,7 +35542,7 @@
         <v>147</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35533,7 +35550,7 @@
         <v>150</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35550,7 +35567,7 @@
         <v>152</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35576,7 +35593,7 @@
         <v>164</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35602,7 +35619,7 @@
         <v>172</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35610,7 +35627,7 @@
         <v>175</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35618,7 +35635,7 @@
         <v>176</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35626,7 +35643,7 @@
         <v>85</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35634,7 +35651,7 @@
         <v>87</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35642,7 +35659,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35650,7 +35667,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35658,7 +35675,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35667,7 +35684,7 @@
         <v>Electricity by biomass and waste</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35676,7 +35693,7 @@
         <v>Electricity by coal</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35685,7 +35702,7 @@
         <v>Electricity by gas</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35694,7 +35711,7 @@
         <v>Electricity by hydro</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35703,7 +35720,7 @@
         <v>Electricity by nuclear</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35712,7 +35729,7 @@
         <v>Electricity by petroleum and other oil derivatives</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35721,7 +35738,7 @@
         <v>Electricity by solar photovoltaic</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35729,7 +35746,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35738,7 +35755,7 @@
         <v>Electricity by wind</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35746,7 +35763,7 @@
         <v>61</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35754,7 +35771,7 @@
         <v>97</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35762,7 +35779,7 @@
         <v>99</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35770,7 +35787,7 @@
         <v>100</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35778,7 +35795,7 @@
         <v>108</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35786,7 +35803,7 @@
         <v>109</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35794,7 +35811,7 @@
         <v>110</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35802,7 +35819,7 @@
         <v>115</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35810,7 +35827,7 @@
         <v>126</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35818,7 +35835,7 @@
         <v>129</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35826,7 +35843,7 @@
         <v>139</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35834,7 +35851,7 @@
         <v>140</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35842,7 +35859,7 @@
         <v>153</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35850,7 +35867,7 @@
         <v>155</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35858,7 +35875,7 @@
         <v>160</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35866,7 +35883,7 @@
         <v>163</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35874,7 +35891,7 @@
         <v>169</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35882,7 +35899,7 @@
         <v>171</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35890,7 +35907,7 @@
         <v>174</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35898,7 +35915,7 @@
         <v>179</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35906,7 +35923,7 @@
         <v>138</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35914,7 +35931,7 @@
         <v>137</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>